<commit_message>
Test funcitons in test.py
</commit_message>
<xml_diff>
--- a/euler_rk4.xlsx
+++ b/euler_rk4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\E-Learning\E-Learning_5th\Math Modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Greenhouse-Dynamic-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{69E888DF-1FBD-4043-9672-44E97F5925BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97335A6-F3E7-452E-9571-0D25E02B7167}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D12B3259-5ACA-4A47-B749-22C5D1F65022}"/>
+    <workbookView xWindow="-7140" yWindow="1425" windowWidth="14955" windowHeight="15375" xr2:uid="{D12B3259-5ACA-4A47-B749-22C5D1F65022}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,14 +414,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CD9A5D8-41EF-4987-B5FB-F0BEFCB05756}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="254" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>